<commit_message>
Update to the latest version of ACMO foramt
Since DSSAT 46 is not available to output EPCP and ESCP, the column for
those two variable are still blank in the sample file
</commit_message>
<xml_diff>
--- a/Temlpates/ACMO/ACMO_templates.xlsx
+++ b/Temlpates/ACMO/ACMO_templates.xlsx
@@ -1244,16 +1244,16 @@
     <t>Unique hash assigned when rotational analysis DOME files are loaded into ACE database</t>
   </si>
   <si>
-    <t>EPCM_S</t>
-  </si>
-  <si>
-    <t>ESCM_S</t>
-  </si>
-  <si>
-    <t>Total season transpiration</t>
-  </si>
-  <si>
-    <t>Total season soil evaporation</t>
+    <t>EPCP_S</t>
+  </si>
+  <si>
+    <t>ESCP_S</t>
+  </si>
+  <si>
+    <t>Transpiration, cumulative from planting to harvest</t>
+  </si>
+  <si>
+    <t>Evaporation,soil, cumulative from planting to harvest</t>
   </si>
 </sst>
 </file>
@@ -2408,10 +2408,10 @@
   <dimension ref="A1:BF82"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="6" ySplit="3" topLeftCell="G4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="3" topLeftCell="AT4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G4" sqref="G4"/>
+      <selection pane="bottomRight" activeCell="BE1" sqref="BE1:BF1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -9975,8 +9975,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2"/>
@@ -10682,7 +10682,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="13.8" thickBot="1">
+    <row r="57" spans="1:4" ht="27" thickBot="1">
       <c r="A57" s="55" t="s">
         <v>386</v>
       </c>
@@ -10696,7 +10696,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="13.8" thickBot="1">
+    <row r="58" spans="1:4" ht="27" thickBot="1">
       <c r="A58" s="55" t="s">
         <v>387</v>
       </c>

</xml_diff>